<commit_message>
fixed code in Syntax to be more consistent with Consistency, retested
</commit_message>
<xml_diff>
--- a/AEF_files/10.syntax.passed/202504251541---Thailand AEF_2024.syntax_checked.xlsx
+++ b/AEF_files/10.syntax.passed/202504251541---Thailand AEF_2024.syntax_checked.xlsx
@@ -4913,17 +4913,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3C6967A-0387-445B-9288-191B53309DA4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBE7325D-D20D-452C-926E-120CCE76722B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C330C2B2-E006-41D7-9AB3-205FD5A6772D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0723B6A8-39F9-457F-8B84-9CD5E60B232F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ABC53B2-5C1F-4191-ABA4-6AA19037ABD8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B70B8623-E534-4D13-986A-C322AEDD7AFA}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC02A60-7DF9-4F84-964B-A882479A30AF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AAFBB15-0A4C-4564-A99A-8A5A76B9DADE}"/>
 </file>
</xml_diff>